<commit_message>
Options two choose when entering client info
</commit_message>
<xml_diff>
--- a/Selenium_project_demo/data/ClientList.xlsx
+++ b/Selenium_project_demo/data/ClientList.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ontariogov-my.sharepoint.com/personal/adnan_faizi_ontario_ca/Documents/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FDA7C1F-0F4C-408C-9537-60B14153D92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1FE14FA4-A161-4305-B258-AD9228BE6217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3A0189A1-E3EB-4CF7-8D17-2234585B8DC7}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="20760" windowHeight="14775" xr2:uid="{3A0189A1-E3EB-4CF7-8D17-2234585B8DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -86,7 +82,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="dd\-mmm\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -120,7 +116,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,12 +434,13 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="3" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>